<commit_message>
chore: stop_word 단어 추가
</commit_message>
<xml_diff>
--- a/ai/stop_words.xlsx
+++ b/ai/stop_words.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSAFY\2학기\특화PJT\ai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSAFY\2학기\특화PJT\특화PJT\ai\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="820">
   <si>
     <t>이</t>
   </si>
@@ -2127,6 +2127,448 @@
   </si>
   <si>
     <t>로그</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>등에</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>너와</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>곳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>후</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뒤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>밖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>옆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>르</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>디</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>줄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>심</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>곁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>짐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>복</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>멍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>덕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>히</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>폰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현</t>
+  </si>
+  <si>
+    <t>창</t>
+  </si>
+  <si>
+    <t>곡</t>
+  </si>
+  <si>
+    <t>북</t>
+  </si>
+  <si>
+    <t>탓</t>
+  </si>
+  <si>
+    <t>밭</t>
+  </si>
+  <si>
+    <t>루</t>
+  </si>
+  <si>
+    <t>혼</t>
+  </si>
+  <si>
+    <t>답</t>
+  </si>
+  <si>
+    <t>똥</t>
+  </si>
+  <si>
+    <t>옥</t>
+  </si>
+  <si>
+    <t>화</t>
+  </si>
+  <si>
+    <t>생</t>
+  </si>
+  <si>
+    <t>양</t>
+  </si>
+  <si>
+    <t>걸</t>
+  </si>
+  <si>
+    <t>업</t>
+  </si>
+  <si>
+    <t>움</t>
+  </si>
+  <si>
+    <t>짓</t>
+  </si>
+  <si>
+    <t>누</t>
+  </si>
+  <si>
+    <t>금</t>
+  </si>
+  <si>
+    <t>깨</t>
+  </si>
+  <si>
+    <t>임</t>
+  </si>
+  <si>
+    <t>부</t>
+  </si>
+  <si>
+    <t>떼</t>
+  </si>
+  <si>
+    <t>군</t>
+  </si>
+  <si>
+    <t>바</t>
+  </si>
+  <si>
+    <t>실</t>
+  </si>
+  <si>
+    <t>끼</t>
+  </si>
+  <si>
+    <t>토</t>
+  </si>
+  <si>
+    <t>단</t>
+  </si>
+  <si>
+    <t>킹</t>
+  </si>
+  <si>
+    <t>공</t>
+  </si>
+  <si>
+    <t>석</t>
+  </si>
+  <si>
+    <t>백</t>
+  </si>
+  <si>
+    <t>님</t>
+  </si>
+  <si>
+    <t>품</t>
+  </si>
+  <si>
+    <t>악</t>
+  </si>
+  <si>
+    <t>렉</t>
+  </si>
+  <si>
+    <t>편</t>
+  </si>
+  <si>
+    <t>난</t>
+  </si>
+  <si>
+    <t>엘</t>
+  </si>
+  <si>
+    <t>맘</t>
+  </si>
+  <si>
+    <t>파</t>
+  </si>
+  <si>
+    <t>조</t>
+  </si>
+  <si>
+    <t>도</t>
+  </si>
+  <si>
+    <t>빅</t>
+  </si>
+  <si>
+    <t>진</t>
+  </si>
+  <si>
+    <t>락</t>
+  </si>
+  <si>
+    <t>용</t>
+  </si>
+  <si>
+    <t>뷰</t>
+  </si>
+  <si>
+    <t>콘</t>
+  </si>
+  <si>
+    <t>볕</t>
+  </si>
+  <si>
+    <t>포</t>
+  </si>
+  <si>
+    <t>샷</t>
+  </si>
+  <si>
+    <t>담</t>
+  </si>
+  <si>
+    <t>콕</t>
+  </si>
+  <si>
+    <t>국</t>
+  </si>
+  <si>
+    <t>카</t>
+  </si>
+  <si>
+    <t>테</t>
+  </si>
+  <si>
+    <t>층</t>
+  </si>
+  <si>
+    <t>암</t>
+  </si>
+  <si>
+    <t>함</t>
+  </si>
+  <si>
+    <t>경</t>
+  </si>
+  <si>
+    <t>터</t>
+  </si>
+  <si>
+    <t>봉</t>
+  </si>
+  <si>
+    <t>서</t>
+  </si>
+  <si>
+    <t>통</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2173,10 +2615,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -2491,10 +2934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C677"/>
+  <dimension ref="A1:C806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A664" workbookViewId="0">
-      <selection activeCell="A677" sqref="A677"/>
+    <sheetView tabSelected="1" topLeftCell="A780" workbookViewId="0">
+      <selection activeCell="B792" sqref="B792"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -6490,6 +6933,651 @@
         <v>692</v>
       </c>
     </row>
+    <row r="678" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A678" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="679" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A679" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="680" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A680" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="681" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A681" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="682" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A682" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="683" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A683" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="684" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A684" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="685" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A685" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="686" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A686" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="687" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A687" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="688" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A688" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="689" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A689" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="690" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A690" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="691" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A691" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="692" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A692" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="693" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A693" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="694" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A694" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="695" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A695" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="696" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A696" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="697" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A697" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="698" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A698" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="699" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A699" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="700" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A700" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="701" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A701" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="702" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A702" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="703" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A703" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="704" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A704" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="705" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A705" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="706" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A706" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="707" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A707" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="708" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A708" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="709" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A709" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="710" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A710" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="711" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A711" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="712" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A712" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="713" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A713" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="714" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A714" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="715" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A715" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="716" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A716" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="717" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A717" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="718" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A718" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="719" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A719" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="720" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A720" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="721" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A721" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="722" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A722" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="723" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A723" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="724" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A724" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="725" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A725" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="726" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A726" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="727" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A727" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="728" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A728" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="729" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A729" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="730" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A730" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="731" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A731" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="732" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A732" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="733" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A733" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="734" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A734" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="735" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A735" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="736" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A736" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="737" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A737" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="738" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A738" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="739" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A739" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="740" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A740" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="741" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A741" s="1" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="742" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A742" s="1" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="743" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A743" s="1" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="744" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A744" s="1" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="745" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A745" s="1" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="746" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A746" s="1" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="747" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A747" s="1" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="748" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A748" s="1" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="749" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A749" s="1" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="750" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A750" s="1" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="751" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A751" s="1" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="752" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A752" s="1" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="753" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A753" s="1" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="754" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A754" s="1" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="755" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A755" s="1" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="756" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A756" s="1" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="757" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A757" s="1" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="758" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A758" s="1" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="759" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A759" s="1" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="760" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A760" s="1" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="761" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A761" s="1" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="762" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A762" s="1" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="763" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A763" s="1" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="764" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A764" s="1" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="765" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A765" s="1" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="766" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A766" s="1" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="767" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A767" s="1" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="768" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A768" s="1" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="769" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A769" s="1" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="770" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A770" s="1" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="771" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A771" s="1" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="772" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A772" s="1" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="773" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A773" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="774" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A774" s="1" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="775" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A775" s="1" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="776" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A776" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="777" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A777" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="778" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A778" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="779" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A779" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="780" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A780" s="1" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="781" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A781" s="1" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="782" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A782" s="1" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="783" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A783" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="784" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A784" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="785" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A785" s="1" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="786" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A786" s="1" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="787" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A787" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="788" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A788" s="1" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="789" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A789" s="1" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="790" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A790" s="1" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="791" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A791" s="1" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="792" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A792" s="1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="793" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A793" s="1" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="794" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A794" s="1" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="795" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A795" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="796" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A796" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="797" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A797" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="798" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A798" s="1" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="799" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A799" s="1" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="800" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A800" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="801" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A801" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="802" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A802" s="1" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="803" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A803" s="1" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="804" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A804" s="1" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="805" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A805" s="1" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="806" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A806" s="1" t="s">
+        <v>818</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>